<commit_message>
develop excel with vba for ingridiens for bake cake
</commit_message>
<xml_diff>
--- a/ciasta.xlsx
+++ b/ciasta.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\excel_VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8806455E-C17D-4845-85F6-093F4DE4918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063E4326-D144-423E-A9BA-6E0F10FA2056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="formularz" sheetId="2" r:id="rId2"/>
+    <sheet name="ustawienia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -85,20 +86,20 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>400050</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>590550</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:col>19</xdr:col>
+          <xdr:colOff>523875</xdr:colOff>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="CommandButton1" hidden="1">
+            <xdr:cNvPr id="1025" name="Button1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
@@ -408,7 +409,9 @@
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -418,19 +421,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId3" name="CommandButton1">
+        <control shapeId="1025" r:id="rId3" name="Button1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>400050</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>590550</xdr:colOff>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>142875</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:col>19</xdr:col>
+                <xdr:colOff>523875</xdr:colOff>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
@@ -438,7 +441,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId3" name="CommandButton1"/>
+        <control shapeId="1025" r:id="rId3" name="Button1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -448,6 +451,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FFE55C-3218-40CC-8D93-729A1156EC74}">
   <sheetPr codeName="Arkusz2"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B57" sqref="B56:B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD30115-9E4A-419D-A966-802320B10EDC}">
+  <sheetPr codeName="Arkusz3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>